<commit_message>
Excel - course for Business Users
</commit_message>
<xml_diff>
--- a/01-СуммЕсли--СуммЕслиМн--СрзначЕсли-СрзначЕслиМн/1-Сумм-срзнач-мин-макс.xlsx
+++ b/01-СуммЕсли--СуммЕслиМн--СрзначЕсли-СрзначЕслиМн/1-Сумм-срзнач-мин-макс.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Excel - Course\01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Excel - Course\01-СуммЕсли--СуммЕслиМн--СрзначЕсли-СрзначЕслиМн\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Стул</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>сред значен</t>
+  </si>
+  <si>
+    <t>ФОРМУЛА =СРЗНАЧ(B2:B9)</t>
+  </si>
+  <si>
+    <t>ФОРМУЛА =(B2-(B2*C2))*D2</t>
   </si>
 </sst>
 </file>
@@ -556,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -572,7 +578,7 @@
     <col min="6" max="11" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -589,7 +595,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -610,8 +616,11 @@
         <f>B2*C2</f>
         <v>1800</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -633,7 +642,7 @@
         <v>3325.0000000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -655,7 +664,7 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -677,7 +686,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -699,7 +708,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -721,7 +730,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -743,7 +752,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -765,7 +774,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
@@ -786,7 +795,7 @@
         <v>1254750</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
@@ -799,7 +808,7 @@
         <v>0.05</v>
       </c>
       <c r="D11" s="6">
-        <f t="shared" ref="C11:E11" si="2">MIN(D2:D9)</f>
+        <f t="shared" ref="D11:E11" si="2">MIN(D2:D9)</f>
         <v>1</v>
       </c>
       <c r="E11" s="6">
@@ -807,7 +816,7 @@
         <v>14400</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>15</v>
       </c>
@@ -828,13 +837,16 @@
         <v>408000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="6">
         <f>AVERAGE(B2:B9)</f>
         <v>65125</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>